<commit_message>
Updates to Batching and Profiles
Accuracy and Evasion are now agent properties with ranges.
</commit_message>
<xml_diff>
--- a/Unity/PathOS/Assets/PathOS+/Agent Configs/agents-template.xlsx
+++ b/Unity/PathOS/Assets/PathOS+/Agent Configs/agents-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samantha\Documents\PathOS\Unity\PathOS\Assets\PathOS\Agent Configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity Projects\pathos-a11y\Unity\PathOS\Assets\PathOS+\Agent Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D97BB5B-E82B-494F-9E01-BA11BB91E0A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CF3C92-CE57-4028-9770-64E4C57610E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10680" yWindow="5025" windowWidth="21600" windowHeight="11385" xr2:uid="{D7DDAED4-DFFF-4F29-92B8-7CD18797808F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D7DDAED4-DFFF-4F29-92B8-7CD18797808F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Experience</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>…</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Evasion</t>
   </si>
 </sst>
 </file>
@@ -409,41 +415,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97244B2E-E60E-4ED6-8095-EA09A87F42A9}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -468,8 +480,14 @@
       <c r="H2">
         <v>0</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -494,8 +512,14 @@
       <c r="H3">
         <v>0</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -518,6 +542,12 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>